<commit_message>
FSV:3.0000, V:4.0.0.0 - add commands and results
</commit_message>
<xml_diff>
--- a/Math/Results_20190626.xlsx
+++ b/Math/Results_20190626.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\ClmFSharp\Math\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF78CA9A-53E9-46A7-9094-C0F9BCA0DA90}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C6B7CE-9244-4BE2-94C3-3BBF8B9AEB6C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="11934" activeTab="7" xr2:uid="{F30BEC68-5FC4-4FD1-AF5F-E57D6551BD0B}"/>
   </bookViews>
@@ -728,13 +728,13 @@
                   <c:v>0.14195692025664527</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.19593173092094882</c:v>
+                  <c:v>0.20893379213991872</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.16042275749657187</c:v>
+                  <c:v>0.15786994602301663</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.40601739304779333</c:v>
+                  <c:v>0.40487255459047</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -769,13 +769,13 @@
                   <c:v>0.20893379213991872</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.28978551654549684</c:v>
+                  <c:v>0.28517415215398717</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.40297793071330623</c:v>
+                  <c:v>0.39656533251858644</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.44763739946380693</c:v>
+                  <c:v>0.44292353275428198</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -810,13 +810,13 @@
                   <c:v>0.27361517166438126</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.39316520275600902</c:v>
+                  <c:v>0.40297793071330623</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.4022502003870892</c:v>
+                  <c:v>0.39739454573547589</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.53037593254112902</c:v>
+                  <c:v>0.54439280785778066</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -848,16 +848,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.25699253967096797</c:v>
+                  <c:v>0.23022137263365605</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.40887220237661298</c:v>
+                  <c:v>0.41755621397840731</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.44602230666732468</c:v>
+                  <c:v>0.41755621397840731</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.60024428761782556</c:v>
+                  <c:v>0.59512744540953</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1226,7 +1226,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3.7780085599194359E-2</c:v>
+                  <c:v>3.3792152226538301E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>6.2391791424788678E-2</c:v>
@@ -1238,10 +1238,10 @@
                   <c:v>0.16338328226733051</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.29936438637603924</c:v>
+                  <c:v>0.26249788887012326</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.11420943798030923</c:v>
+                  <c:v>0.10416314811687213</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1310,22 +1310,22 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>5.6340853677355633E-2</c:v>
+                  <c:v>6.8977650171705207E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.11013086872390264</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.17659310237768752</c:v>
+                  <c:v>0.17378297178938795</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.16882153454853752</c:v>
+                  <c:v>0.19212689297978941</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.19513154582074524</c:v>
+                  <c:v>0.17453414400720596</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.7449018126888213E-2</c:v>
+                  <c:v>5.1384901199121757E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1367,22 +1367,22 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>9.4120939276549992E-2</c:v>
+                  <c:v>0.10276980239824351</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.17252266014869133</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.31663511159261204</c:v>
+                  <c:v>0.3138249810043125</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.332204816815868</c:v>
+                  <c:v>0.35551017524711992</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.49449593219678445</c:v>
+                  <c:v>0.43703203287732922</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.17165845610719743</c:v>
+                  <c:v>0.15554804931599389</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1430,13 +1430,13 @@
                   <c:v>0.14195692025664527</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.28978551654549684</c:v>
+                  <c:v>0.28517415215398717</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.4022502003870892</c:v>
+                  <c:v>0.39739454573547589</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.60024428761782556</c:v>
+                  <c:v>0.59512744540953</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.5</c:v>
@@ -10171,7 +10171,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA892EB-1C5D-4DA9-95FA-D6E2F64A7CF0}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -11200,16 +11202,16 @@
         <v>15028</v>
       </c>
       <c r="C32">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="D32">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E32" s="1">
-        <v>0.75</v>
+        <v>0.58330000000000004</v>
       </c>
       <c r="F32" s="2">
-        <v>0.65</v>
+        <v>1.82</v>
       </c>
       <c r="G32">
         <v>10</v>
@@ -11671,7 +11673,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53871AB-6ECF-45F9-A8A5-AF6AEDD22179}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -12671,7 +12675,7 @@
         <v>11001</v>
       </c>
       <c r="C31">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -12680,7 +12684,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="2">
-        <v>1.35</v>
+        <v>1.42</v>
       </c>
       <c r="G31">
         <v>0.1</v>
@@ -12700,16 +12704,16 @@
         <v>11002</v>
       </c>
       <c r="C32">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32" s="1">
-        <v>9.0899999999999995E-2</v>
+        <v>5.5599999999999997E-2</v>
       </c>
       <c r="F32" s="2">
-        <v>2.09</v>
+        <v>1.92</v>
       </c>
       <c r="G32">
         <v>0.1</v>
@@ -12729,16 +12733,16 @@
         <v>11003</v>
       </c>
       <c r="C33">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D33">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E33" s="1">
-        <v>0.18179999999999999</v>
+        <v>0.27779999999999999</v>
       </c>
       <c r="F33" s="2">
-        <v>1.22</v>
+        <v>1.31</v>
       </c>
       <c r="G33">
         <v>0.1</v>
@@ -12758,16 +12762,16 @@
         <v>11004</v>
       </c>
       <c r="C34">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E34" s="1">
-        <v>9.0899999999999995E-2</v>
+        <v>0.22220000000000001</v>
       </c>
       <c r="F34" s="2">
-        <v>1.52</v>
+        <v>1.42</v>
       </c>
       <c r="G34">
         <v>0.1</v>
@@ -12787,16 +12791,16 @@
         <v>11005</v>
       </c>
       <c r="C35">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35" s="1">
-        <v>8.3299999999999999E-2</v>
+        <v>0.1111</v>
       </c>
       <c r="F35" s="2">
-        <v>1.06</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="G35">
         <v>0.1</v>
@@ -12816,16 +12820,16 @@
         <v>12001</v>
       </c>
       <c r="C36">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E36" s="1">
-        <v>9.0899999999999995E-2</v>
+        <v>0.1111</v>
       </c>
       <c r="F36" s="2">
-        <v>1.44</v>
+        <v>1.49</v>
       </c>
       <c r="G36">
         <v>0.1</v>
@@ -12845,16 +12849,16 @@
         <v>12002</v>
       </c>
       <c r="C37">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D37">
         <v>3</v>
       </c>
       <c r="E37" s="1">
-        <v>0.25</v>
+        <v>0.16669999999999999</v>
       </c>
       <c r="F37" s="2">
-        <v>1.27</v>
+        <v>1.21</v>
       </c>
       <c r="G37">
         <v>0.1</v>
@@ -12874,16 +12878,16 @@
         <v>12003</v>
       </c>
       <c r="C38">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38" s="1">
-        <v>9.0899999999999995E-2</v>
+        <v>5.5599999999999997E-2</v>
       </c>
       <c r="F38" s="2">
-        <v>1.49</v>
+        <v>1.46</v>
       </c>
       <c r="G38">
         <v>0.1</v>
@@ -12903,16 +12907,16 @@
         <v>12004</v>
       </c>
       <c r="C39">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" s="1">
-        <v>0</v>
+        <v>5.5599999999999997E-2</v>
       </c>
       <c r="F39" s="2">
-        <v>1.23</v>
+        <v>1.34</v>
       </c>
       <c r="G39">
         <v>0.1</v>
@@ -12932,16 +12936,16 @@
         <v>12005</v>
       </c>
       <c r="C40">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E40" s="1">
-        <v>9.0899999999999995E-2</v>
+        <v>0.17649999999999999</v>
       </c>
       <c r="F40" s="2">
-        <v>1.79</v>
+        <v>1.74</v>
       </c>
       <c r="G40">
         <v>0.1</v>
@@ -12961,16 +12965,16 @@
         <v>13000</v>
       </c>
       <c r="C41">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41" s="1">
-        <v>0</v>
+        <v>5.5599999999999997E-2</v>
       </c>
       <c r="F41" s="2">
-        <v>1.7</v>
+        <v>1.62</v>
       </c>
       <c r="G41">
         <v>0.1</v>
@@ -12990,16 +12994,16 @@
         <v>13001</v>
       </c>
       <c r="C42">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D42">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E42" s="1">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="F42" s="2">
-        <v>1.92</v>
+        <v>1.77</v>
       </c>
       <c r="G42">
         <v>1</v>
@@ -13019,16 +13023,16 @@
         <v>13002</v>
       </c>
       <c r="C43">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D43">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E43" s="1">
-        <v>0.33329999999999999</v>
+        <v>0.3125</v>
       </c>
       <c r="F43" s="2">
-        <v>2.4300000000000002</v>
+        <v>2.41</v>
       </c>
       <c r="G43">
         <v>10</v>
@@ -13048,13 +13052,13 @@
         <v>14000</v>
       </c>
       <c r="C44">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E44" s="1">
-        <v>0.1</v>
+        <v>0.1176</v>
       </c>
       <c r="F44" s="2">
         <v>1.47</v>
@@ -13077,16 +13081,16 @@
         <v>14001</v>
       </c>
       <c r="C45">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E45" s="1">
-        <v>9.0899999999999995E-2</v>
+        <v>0.1176</v>
       </c>
       <c r="F45" s="2">
-        <v>1.06</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="G45">
         <v>1</v>
@@ -13106,16 +13110,16 @@
         <v>14002</v>
       </c>
       <c r="C46">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="D46">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E46" s="1">
-        <v>0.3</v>
+        <v>0.35289999999999999</v>
       </c>
       <c r="F46" s="2">
-        <v>1.54</v>
+        <v>1.69</v>
       </c>
       <c r="G46">
         <v>10</v>
@@ -13435,16 +13439,16 @@
         <v>7003</v>
       </c>
       <c r="C3">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D3">
         <v>8</v>
       </c>
       <c r="E3" s="1">
-        <v>0.33329999999999999</v>
+        <v>0.32</v>
       </c>
       <c r="F3" s="2">
-        <v>5.34</v>
+        <v>5.4</v>
       </c>
       <c r="G3">
         <v>0.1</v>
@@ -13464,7 +13468,7 @@
         <v>7004</v>
       </c>
       <c r="C4">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -13473,7 +13477,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="2">
-        <v>5.32</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="G4">
         <v>0.1</v>
@@ -13493,16 +13497,16 @@
         <v>7005</v>
       </c>
       <c r="C5">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5" s="1">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="F5" s="2">
-        <v>4.58</v>
+        <v>4.43</v>
       </c>
       <c r="G5">
         <v>0.1</v>
@@ -13522,16 +13526,16 @@
         <v>7006</v>
       </c>
       <c r="C6">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D6">
         <v>4</v>
       </c>
       <c r="E6" s="1">
-        <v>0.22220000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="F6" s="2">
-        <v>6.64</v>
+        <v>5.56</v>
       </c>
       <c r="G6">
         <v>0.1</v>
@@ -13551,16 +13555,16 @@
         <v>9000</v>
       </c>
       <c r="C7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7">
         <v>5</v>
       </c>
       <c r="E7" s="1">
-        <v>0.20830000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="F7" s="2">
-        <v>5.73</v>
+        <v>5.78</v>
       </c>
       <c r="G7">
         <v>0.1</v>
@@ -13621,16 +13625,16 @@
         <v>9002</v>
       </c>
       <c r="C9">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D9">
         <v>5</v>
       </c>
       <c r="E9" s="1">
-        <v>0.20830000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="F9" s="2">
-        <v>5.74</v>
+        <v>5.66</v>
       </c>
       <c r="G9">
         <v>0.1</v>
@@ -13656,16 +13660,16 @@
         <v>9003</v>
       </c>
       <c r="C10">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E10" s="1">
-        <v>0.125</v>
+        <v>0.16</v>
       </c>
       <c r="F10" s="2">
-        <v>5.18</v>
+        <v>6.95</v>
       </c>
       <c r="G10">
         <v>0.1</v>
@@ -13726,16 +13730,16 @@
         <v>9005</v>
       </c>
       <c r="C12">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D12">
         <v>5</v>
       </c>
       <c r="E12" s="1">
-        <v>0.20830000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="F12" s="2">
-        <v>4.22</v>
+        <v>4.41</v>
       </c>
       <c r="G12">
         <v>0.1</v>
@@ -13761,16 +13765,16 @@
         <v>9006</v>
       </c>
       <c r="C13">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D13">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E13" s="1">
-        <v>0.5</v>
+        <v>0.52</v>
       </c>
       <c r="F13" s="2">
-        <v>4.7699999999999996</v>
+        <v>5.95</v>
       </c>
       <c r="G13">
         <v>0.1</v>
@@ -13831,16 +13835,16 @@
         <v>9008</v>
       </c>
       <c r="C15">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D15">
         <v>8</v>
       </c>
       <c r="E15" s="1">
-        <v>0.33329999999999999</v>
+        <v>0.32</v>
       </c>
       <c r="F15" s="2">
-        <v>5.55</v>
+        <v>5.67</v>
       </c>
       <c r="G15">
         <v>0.1</v>
@@ -13866,16 +13870,16 @@
         <v>9010</v>
       </c>
       <c r="C16">
+        <v>25</v>
+      </c>
+      <c r="D16">
         <v>13</v>
       </c>
-      <c r="D16">
-        <v>8</v>
-      </c>
       <c r="E16" s="1">
-        <v>0.61539999999999995</v>
+        <v>0.52</v>
       </c>
       <c r="F16" s="2">
-        <v>7.22</v>
+        <v>5</v>
       </c>
       <c r="G16">
         <v>0.1</v>
@@ -13901,16 +13905,16 @@
         <v>9013</v>
       </c>
       <c r="C17">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E17" s="1">
-        <v>0.2</v>
+        <v>0.32</v>
       </c>
       <c r="F17" s="2">
-        <v>8.1199999999999992</v>
+        <v>5.41</v>
       </c>
       <c r="G17">
         <v>0.1</v>
@@ -13936,16 +13940,16 @@
         <v>9016</v>
       </c>
       <c r="C18">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D18">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E18" s="1">
-        <v>0.66669999999999996</v>
+        <v>0.64</v>
       </c>
       <c r="F18" s="2">
-        <v>7.36</v>
+        <v>5.15</v>
       </c>
       <c r="G18">
         <v>0.1</v>
@@ -13971,16 +13975,16 @@
         <v>9025</v>
       </c>
       <c r="C19">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E19" s="1">
-        <v>0.25</v>
+        <v>0.16669999999999999</v>
       </c>
       <c r="F19" s="2">
-        <v>7.22</v>
+        <v>5.12</v>
       </c>
       <c r="G19">
         <v>0.1</v>
@@ -14006,16 +14010,16 @@
         <v>9026</v>
       </c>
       <c r="C20">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D20">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E20" s="1">
-        <v>0.58330000000000004</v>
+        <v>0.52</v>
       </c>
       <c r="F20" s="2">
-        <v>7.3</v>
+        <v>5.2</v>
       </c>
       <c r="G20">
         <v>0.1</v>
@@ -14041,16 +14045,16 @@
         <v>9027</v>
       </c>
       <c r="C21">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="D21">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E21" s="1">
-        <v>0.36359999999999998</v>
+        <v>0.32</v>
       </c>
       <c r="F21" s="2">
-        <v>7.96</v>
+        <v>5.93</v>
       </c>
       <c r="G21">
         <v>0.1</v>
@@ -14076,16 +14080,16 @@
         <v>9028</v>
       </c>
       <c r="C22">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="D22">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E22" s="1">
-        <v>0.45450000000000002</v>
+        <v>0.52</v>
       </c>
       <c r="F22" s="2">
-        <v>7.98</v>
+        <v>5.45</v>
       </c>
       <c r="G22">
         <v>0.1</v>
@@ -14111,16 +14115,16 @@
         <v>10000</v>
       </c>
       <c r="C23">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D23">
         <v>2</v>
       </c>
       <c r="E23" s="1">
-        <v>8.3299999999999999E-2</v>
+        <v>0.08</v>
       </c>
       <c r="F23" s="2">
-        <v>5.37</v>
+        <v>5.45</v>
       </c>
       <c r="G23">
         <v>0.1</v>
@@ -14169,16 +14173,16 @@
         <v>10002</v>
       </c>
       <c r="C25">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D25">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E25" s="1">
-        <v>0.1429</v>
+        <v>0.2</v>
       </c>
       <c r="F25" s="2">
-        <v>5.38</v>
+        <v>5.0599999999999996</v>
       </c>
       <c r="G25">
         <v>0.1</v>
@@ -14198,16 +14202,16 @@
         <v>10003</v>
       </c>
       <c r="C26">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D26">
         <v>4</v>
       </c>
       <c r="E26" s="1">
-        <v>0.21049999999999999</v>
+        <v>0.16</v>
       </c>
       <c r="F26" s="2">
-        <v>6.55</v>
+        <v>5.66</v>
       </c>
       <c r="G26">
         <v>0.1</v>
@@ -14227,16 +14231,16 @@
         <v>10004</v>
       </c>
       <c r="C27">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="1">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="F27" s="2">
-        <v>6.4</v>
+        <v>5.93</v>
       </c>
       <c r="G27">
         <v>0.1</v>
@@ -14256,16 +14260,16 @@
         <v>10005</v>
       </c>
       <c r="C28">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28" s="1">
-        <v>5.2600000000000001E-2</v>
+        <v>0.04</v>
       </c>
       <c r="F28" s="2">
-        <v>6.19</v>
+        <v>5.59</v>
       </c>
       <c r="G28">
         <v>0.1</v>
@@ -14286,8 +14290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8FF1825-D8E5-4ED0-A241-603EC8F66EAC}">
   <dimension ref="A1:AI36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE3" sqref="AE3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -14420,15 +14424,15 @@
       </c>
       <c r="AB3" s="83">
         <f>+F16</f>
-        <v>0.19593173092094882</v>
+        <v>0.20893379213991872</v>
       </c>
       <c r="AC3" s="83">
         <f>+F18</f>
-        <v>0.16042275749657187</v>
+        <v>0.15786994602301663</v>
       </c>
       <c r="AD3" s="83">
         <f>+F23</f>
-        <v>0.40601739304779333</v>
+        <v>0.40487255459047</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.55000000000000004">
@@ -14475,15 +14479,15 @@
       </c>
       <c r="AB4" s="90">
         <f>+F13</f>
-        <v>0.28978551654549684</v>
+        <v>0.28517415215398717</v>
       </c>
       <c r="AC4" s="90">
         <f>+F15</f>
-        <v>0.40297793071330623</v>
+        <v>0.39656533251858644</v>
       </c>
       <c r="AD4" s="90">
         <f>+F22</f>
-        <v>0.44763739946380693</v>
+        <v>0.44292353275428198</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.55000000000000004">
@@ -14495,7 +14499,7 @@
       </c>
       <c r="C5" s="36">
         <f>IFERROR(VLOOKUP($B5, ZEN!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B5, ZEN_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B5, CLM!$B$2:$D$101, 2,FALSE), 0)+ IFERROR(VLOOKUP($B5, CLM_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B5, THUNDER!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B5, THUNDER_3200!$B$2:$D$101, 2,FALSE), 0)</f>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D5" s="36">
         <f>IFERROR(VLOOKUP($B5, ZEN!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B5, ZEN_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B5, CLM!$B$2:$D$101, 3,FALSE), 0)+ IFERROR(VLOOKUP($B5, CLM_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B5, THUNDER!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B5, THUNDER_3200!$B$2:$D$101, 3,FALSE), 0)</f>
@@ -14503,23 +14507,23 @@
       </c>
       <c r="E5" s="51">
         <f t="shared" si="0"/>
-        <v>0.31034482758620691</v>
+        <v>0.30508474576271188</v>
       </c>
       <c r="F5" s="51">
         <f>(E5 + Params!$B$3^2/(2 * C5))/(1 + Params!$B$3^2/C5)</f>
-        <v>0.32212620630772809</v>
+        <v>0.31700020368672982</v>
       </c>
       <c r="G5" s="37">
         <f>IFERROR((Params!$B$3/(1+Params!$B$3^2/C5))*SQRT(E5*(1-E5)/C5 + (Params!$B$3/(2*C5))^2), 0)</f>
-        <v>0.11590686215967136</v>
+        <v>0.11446546891070856</v>
       </c>
       <c r="H5" s="37">
         <f t="shared" si="1"/>
-        <v>0.20621934414805673</v>
+        <v>0.20253473477602124</v>
       </c>
       <c r="I5" s="38">
         <f t="shared" si="2"/>
-        <v>0.43803306846739942</v>
+        <v>0.4314656725974384</v>
       </c>
       <c r="Z5" s="101">
         <v>20</v>
@@ -14530,15 +14534,15 @@
       </c>
       <c r="AB5" s="102">
         <f>+F19</f>
-        <v>0.39316520275600902</v>
+        <v>0.40297793071330623</v>
       </c>
       <c r="AC5" s="102">
         <f>+F21</f>
-        <v>0.4022502003870892</v>
+        <v>0.39739454573547589</v>
       </c>
       <c r="AD5" s="102">
         <f>+F24</f>
-        <v>0.53037593254112902</v>
+        <v>0.54439280785778066</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.55000000000000004">
@@ -14550,7 +14554,7 @@
       </c>
       <c r="C6" s="36">
         <f>IFERROR(VLOOKUP($B6, ZEN!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B6, ZEN_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B6, CLM!$B$2:$D$101, 2,FALSE), 0)+ IFERROR(VLOOKUP($B6, CLM_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B6, THUNDER!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B6, THUNDER_3200!$B$2:$D$101, 2,FALSE), 0)</f>
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D6" s="36">
         <f>IFERROR(VLOOKUP($B6, ZEN!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B6, ZEN_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B6, CLM!$B$2:$D$101, 3,FALSE), 0)+ IFERROR(VLOOKUP($B6, CLM_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B6, THUNDER!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B6, THUNDER_3200!$B$2:$D$101, 3,FALSE), 0)</f>
@@ -14562,11 +14566,11 @@
       </c>
       <c r="F6" s="51">
         <f>(E6 + Params!$B$3^2/(2 * C6))/(1 + Params!$B$3^2/C6)</f>
-        <v>3.7780085599194359E-2</v>
+        <v>3.3792152226538301E-2</v>
       </c>
       <c r="G6" s="37">
         <f>IFERROR((Params!$B$3/(1+Params!$B$3^2/C6))*SQRT(E6*(1-E6)/C6 + (Params!$B$3/(2*C6))^2), 0)</f>
-        <v>3.7780085599194359E-2</v>
+        <v>3.3792152226538308E-2</v>
       </c>
       <c r="H6" s="37">
         <f t="shared" si="1"/>
@@ -14574,26 +14578,26 @@
       </c>
       <c r="I6" s="38">
         <f t="shared" si="2"/>
-        <v>7.5560171198388718E-2</v>
+        <v>6.7584304453076616E-2</v>
       </c>
       <c r="Z6" s="103">
         <v>50</v>
       </c>
       <c r="AA6" s="104">
         <f>+F26</f>
-        <v>0.25699253967096797</v>
+        <v>0.23022137263365605</v>
       </c>
       <c r="AB6" s="104">
         <f>+F27</f>
-        <v>0.40887220237661298</v>
+        <v>0.41755621397840731</v>
       </c>
       <c r="AC6" s="104">
         <f>+F28</f>
-        <v>0.44602230666732468</v>
+        <v>0.41755621397840731</v>
       </c>
       <c r="AD6" s="104">
         <f>+F29</f>
-        <v>0.60024428761782556</v>
+        <v>0.59512744540953</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.55000000000000004">
@@ -14605,7 +14609,7 @@
       </c>
       <c r="C7" s="36">
         <f>IFERROR(VLOOKUP($B7, ZEN!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B7, ZEN_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B7, CLM!$B$2:$D$101, 2,FALSE), 0)+ IFERROR(VLOOKUP($B7, CLM_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B7, THUNDER!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B7, THUNDER_3200!$B$2:$D$101, 2,FALSE), 0)</f>
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D7" s="36">
         <f>IFERROR(VLOOKUP($B7, ZEN!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B7, ZEN_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B7, CLM!$B$2:$D$101, 3,FALSE), 0)+ IFERROR(VLOOKUP($B7, CLM_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B7, THUNDER!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B7, THUNDER_3200!$B$2:$D$101, 3,FALSE), 0)</f>
@@ -14613,23 +14617,23 @@
       </c>
       <c r="E7" s="51">
         <f t="shared" si="3"/>
-        <v>8.3333333333333329E-2</v>
+        <v>7.5471698113207544E-2</v>
       </c>
       <c r="F7" s="51">
         <f>(E7 + Params!$B$3^2/(2 * C7))/(1 + Params!$B$3^2/C7)</f>
-        <v>0.11420943798030923</v>
+        <v>0.10416314811687213</v>
       </c>
       <c r="G7" s="37">
         <f>IFERROR((Params!$B$3/(1+Params!$B$3^2/C7))*SQRT(E7*(1-E7)/C7 + (Params!$B$3/(2*C7))^2), 0)</f>
-        <v>8.1326213630353666E-2</v>
+        <v>7.4424074517970326E-2</v>
       </c>
       <c r="H7" s="37">
         <f t="shared" si="1"/>
-        <v>3.2883224349955567E-2</v>
+        <v>2.9739073598901808E-2</v>
       </c>
       <c r="I7" s="38">
         <f t="shared" si="2"/>
-        <v>0.19553565161066289</v>
+        <v>0.17858722263484245</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.55000000000000004">
@@ -14641,7 +14645,7 @@
       </c>
       <c r="C8" s="36">
         <f>IFERROR(VLOOKUP($B8, ZEN!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B8, ZEN_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B8, CLM!$B$2:$D$101, 2,FALSE), 0)+ IFERROR(VLOOKUP($B8, CLM_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B8, THUNDER!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B8, THUNDER_3200!$B$2:$D$101, 2,FALSE), 0)</f>
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D8" s="36">
         <f>IFERROR(VLOOKUP($B8, ZEN!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B8, ZEN_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B8, CLM!$B$2:$D$101, 3,FALSE), 0)+ IFERROR(VLOOKUP($B8, CLM_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B8, THUNDER!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B8, THUNDER_3200!$B$2:$D$101, 3,FALSE), 0)</f>
@@ -14649,23 +14653,23 @@
       </c>
       <c r="E8" s="51">
         <f t="shared" ref="E8" si="4">IFERROR(D8/C8, 0)</f>
-        <v>0.28260869565217389</v>
+        <v>0.24528301886792453</v>
       </c>
       <c r="F8" s="51">
         <f>(E8 + Params!$B$3^2/(2 * C8))/(1 + Params!$B$3^2/C8)</f>
-        <v>0.29936438637603924</v>
+        <v>0.26249788887012326</v>
       </c>
       <c r="G8" s="37">
         <f>IFERROR((Params!$B$3/(1+Params!$B$3^2/C8))*SQRT(E8*(1-E8)/C8 + (Params!$B$3/(2*C8))^2), 0)</f>
-        <v>0.12612397092689853</v>
+        <v>0.11317026175157749</v>
       </c>
       <c r="H8" s="37">
         <f t="shared" si="1"/>
-        <v>0.17324041544914071</v>
+        <v>0.14932762711854577</v>
       </c>
       <c r="I8" s="38">
         <f t="shared" si="2"/>
-        <v>0.42548835730293777</v>
+        <v>0.37566815062170078</v>
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.55000000000000004">
@@ -14807,15 +14811,15 @@
       </c>
       <c r="AA11" s="1">
         <f>+$F$6</f>
-        <v>3.7780085599194359E-2</v>
+        <v>3.3792152226538301E-2</v>
       </c>
       <c r="AB11" s="1">
         <f>+$F$35</f>
-        <v>5.6340853677355633E-2</v>
+        <v>6.8977650171705207E-2</v>
       </c>
       <c r="AC11" s="1">
         <f>+AA11+AB11</f>
-        <v>9.4120939276549992E-2</v>
+        <v>0.10276980239824351</v>
       </c>
       <c r="AD11" s="1">
         <f>+$F$25</f>
@@ -14823,11 +14827,11 @@
       </c>
       <c r="AF11" s="1">
         <f>+$G$6</f>
-        <v>3.7780085599194359E-2</v>
+        <v>3.3792152226538308E-2</v>
       </c>
       <c r="AG11" s="1">
         <f>+$G$35</f>
-        <v>5.2653837697955938E-2</v>
+        <v>5.8567581337885935E-2</v>
       </c>
       <c r="AH11" s="1"/>
       <c r="AI11" s="1">
@@ -14912,7 +14916,7 @@
       </c>
       <c r="C13" s="92">
         <f>IFERROR(VLOOKUP($B13, ZEN!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B13, ZEN_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B13, CLM!$B$2:$D$101, 2,FALSE), 0)+ IFERROR(VLOOKUP($B13, CLM_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B13, THUNDER!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B13, THUNDER_3200!$B$2:$D$101, 2,FALSE), 0)</f>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D13" s="92">
         <f>IFERROR(VLOOKUP($B13, ZEN!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B13, ZEN_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B13, CLM!$B$2:$D$101, 3,FALSE), 0)+ IFERROR(VLOOKUP($B13, CLM_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B13, THUNDER!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B13, THUNDER_3200!$B$2:$D$101, 3,FALSE), 0)</f>
@@ -14920,23 +14924,23 @@
       </c>
       <c r="E13" s="93">
         <f t="shared" si="5"/>
-        <v>0.27586206896551724</v>
+        <v>0.2711864406779661</v>
       </c>
       <c r="F13" s="93">
         <f>(E13 + Params!$B$3^2/(2 * C13))/(1 + Params!$B$3^2/C13)</f>
-        <v>0.28978551654549684</v>
+        <v>0.28517415215398717</v>
       </c>
       <c r="G13" s="94">
         <f>IFERROR((Params!$B$3/(1+Params!$B$3^2/C13))*SQRT(E13*(1-E13)/C13 + (Params!$B$3/(2*C13))^2), 0)</f>
-        <v>0.1122634797380349</v>
+        <v>0.1108059022289038</v>
       </c>
       <c r="H13" s="94">
         <f t="shared" si="1"/>
-        <v>0.17752203680746192</v>
+        <v>0.17436824992508337</v>
       </c>
       <c r="I13" s="95">
         <f t="shared" si="2"/>
-        <v>0.40204899628353175</v>
+        <v>0.39598005438289097</v>
       </c>
       <c r="Z13">
         <v>10</v>
@@ -14947,15 +14951,15 @@
       </c>
       <c r="AB13" s="1">
         <f>+$F$31</f>
-        <v>0.17659310237768752</v>
+        <v>0.17378297178938795</v>
       </c>
       <c r="AC13" s="1">
         <f t="shared" si="6"/>
-        <v>0.31663511159261204</v>
+        <v>0.3138249810043125</v>
       </c>
       <c r="AD13" s="1">
         <f>+$F$13</f>
-        <v>0.28978551654549684</v>
+        <v>0.28517415215398717</v>
       </c>
       <c r="AF13" s="1">
         <f>+$G$2</f>
@@ -14963,12 +14967,12 @@
       </c>
       <c r="AG13" s="1">
         <f>+$G$31</f>
-        <v>9.2749128210185508E-2</v>
+        <v>9.1399260898714321E-2</v>
       </c>
       <c r="AH13" s="1"/>
       <c r="AI13" s="1">
         <f>+$G$13</f>
-        <v>0.1122634797380349</v>
+        <v>0.1108059022289038</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.55000000000000004">
@@ -15015,15 +15019,15 @@
       </c>
       <c r="AB14" s="1">
         <f>+$F$33</f>
-        <v>0.16882153454853752</v>
+        <v>0.19212689297978941</v>
       </c>
       <c r="AC14" s="1">
         <f t="shared" si="6"/>
-        <v>0.332204816815868</v>
+        <v>0.35551017524711992</v>
       </c>
       <c r="AD14" s="1">
         <f>+$F$21</f>
-        <v>0.4022502003870892</v>
+        <v>0.39739454573547589</v>
       </c>
       <c r="AF14" s="1">
         <f>+$G$3</f>
@@ -15031,12 +15035,12 @@
       </c>
       <c r="AG14" s="1">
         <f>+$G$33</f>
-        <v>9.7858197343091674E-2</v>
+        <v>0.10012847525755188</v>
       </c>
       <c r="AH14" s="1"/>
       <c r="AI14" s="1">
         <f>+$G$21</f>
-        <v>0.10613324782920337</v>
+        <v>0.10526756906167181</v>
       </c>
     </row>
     <row r="15" spans="1:35" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -15048,7 +15052,7 @@
       </c>
       <c r="C15" s="97">
         <f>IFERROR(VLOOKUP($B15, ZEN!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B15, ZEN_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B15, CLM!$B$2:$D$101, 2,FALSE), 0)+ IFERROR(VLOOKUP($B15, CLM_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B15, THUNDER!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B15, THUNDER_3200!$B$2:$D$101, 2,FALSE), 0)</f>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D15" s="97">
         <f>IFERROR(VLOOKUP($B15, ZEN!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B15, ZEN_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B15, CLM!$B$2:$D$101, 3,FALSE), 0)+ IFERROR(VLOOKUP($B15, CLM_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B15, THUNDER!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B15, THUNDER_3200!$B$2:$D$101, 3,FALSE), 0)</f>
@@ -15056,55 +15060,55 @@
       </c>
       <c r="E15" s="98">
         <f t="shared" si="5"/>
-        <v>0.39655172413793105</v>
+        <v>0.38983050847457629</v>
       </c>
       <c r="F15" s="98">
         <f>(E15 + Params!$B$3^2/(2 * C15))/(1 + Params!$B$3^2/C15)</f>
-        <v>0.40297793071330623</v>
+        <v>0.39656533251858644</v>
       </c>
       <c r="G15" s="99">
         <f>IFERROR((Params!$B$3/(1+Params!$B$3^2/C15))*SQRT(E15*(1-E15)/C15 + (Params!$B$3/(2*C15))^2), 0)</f>
-        <v>0.1220922412121949</v>
+        <v>0.12077357186274237</v>
       </c>
       <c r="H15" s="99">
         <f t="shared" si="1"/>
-        <v>0.28088568950111131</v>
+        <v>0.2757917606558441</v>
       </c>
       <c r="I15" s="100">
         <f t="shared" si="2"/>
-        <v>0.52507017192550109</v>
+        <v>0.51733890438132879</v>
       </c>
       <c r="Z15">
         <v>50</v>
       </c>
       <c r="AA15" s="1">
         <f>+$F$8</f>
-        <v>0.29936438637603924</v>
+        <v>0.26249788887012326</v>
       </c>
       <c r="AB15" s="1">
         <f>+$F$34</f>
-        <v>0.19513154582074524</v>
+        <v>0.17453414400720596</v>
       </c>
       <c r="AC15" s="1">
         <f t="shared" si="6"/>
-        <v>0.49449593219678445</v>
+        <v>0.43703203287732922</v>
       </c>
       <c r="AD15" s="1">
         <f>+$F$29</f>
-        <v>0.60024428761782556</v>
+        <v>0.59512744540953</v>
       </c>
       <c r="AF15" s="1">
         <f>+$G$8</f>
-        <v>0.12612397092689853</v>
+        <v>0.11317026175157749</v>
       </c>
       <c r="AG15" s="1">
         <f>+$G$34</f>
-        <v>0.10626896490810595</v>
+        <v>9.601090142938945E-2</v>
       </c>
       <c r="AH15" s="1"/>
       <c r="AI15" s="1">
         <f>+$G$29</f>
-        <v>0.11907404376173815</v>
+        <v>0.10824912380876403</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.55000000000000004">
@@ -15116,46 +15120,46 @@
       </c>
       <c r="C16" s="68">
         <f>IFERROR(VLOOKUP($B16, ZEN!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B16, ZEN_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B16, CLM!$B$2:$D$101, 2,FALSE), 0)+ IFERROR(VLOOKUP($B16, CLM_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B16, THUNDER!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B16, THUNDER_3200!$B$2:$D$101, 2,FALSE), 0)</f>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D16" s="68">
         <f>IFERROR(VLOOKUP($B16, ZEN!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B16, ZEN_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B16, CLM!$B$2:$D$101, 3,FALSE), 0)+ IFERROR(VLOOKUP($B16, CLM_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B16, THUNDER!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B16, THUNDER_3200!$B$2:$D$101, 3,FALSE), 0)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E16" s="69">
         <f t="shared" si="5"/>
-        <v>0.17543859649122806</v>
+        <v>0.18965517241379309</v>
       </c>
       <c r="F16" s="69">
         <f>(E16 + Params!$B$3^2/(2 * C16))/(1 + Params!$B$3^2/C16)</f>
-        <v>0.19593173092094882</v>
+        <v>0.20893379213991872</v>
       </c>
       <c r="G16" s="70">
         <f>IFERROR((Params!$B$3/(1+Params!$B$3^2/C16))*SQRT(E16*(1-E16)/C16 + (Params!$B$3/(2*C16))^2), 0)</f>
-        <v>9.7744259584982729E-2</v>
+        <v>9.9592391714244374E-2</v>
       </c>
       <c r="H16" s="70">
         <f t="shared" si="1"/>
-        <v>9.8187471335966087E-2</v>
+        <v>0.10934140042567435</v>
       </c>
       <c r="I16" s="71">
         <f t="shared" si="2"/>
-        <v>0.29367599050593152</v>
+        <v>0.30852618385416308</v>
       </c>
       <c r="Z16">
         <v>100</v>
       </c>
       <c r="AA16" s="1">
         <f>+$F$7</f>
-        <v>0.11420943798030923</v>
+        <v>0.10416314811687213</v>
       </c>
       <c r="AB16" s="1">
         <f>+$F$36</f>
-        <v>5.7449018126888213E-2</v>
+        <v>5.1384901199121757E-2</v>
       </c>
       <c r="AC16" s="1">
         <f t="shared" si="6"/>
-        <v>0.17165845610719743</v>
+        <v>0.15554804931599389</v>
       </c>
       <c r="AD16" s="1">
         <f>+$F$30</f>
@@ -15163,11 +15167,11 @@
       </c>
       <c r="AF16" s="1">
         <f>+$G$7</f>
-        <v>8.1326213630353666E-2</v>
+        <v>7.4424074517970326E-2</v>
       </c>
       <c r="AG16" s="1">
         <f>+$G$36</f>
-        <v>5.3683347116423218E-2</v>
+        <v>4.8046533812372359E-2</v>
       </c>
       <c r="AH16" s="1"/>
       <c r="AI16" s="1">
@@ -15220,7 +15224,7 @@
       </c>
       <c r="C18" s="78">
         <f>IFERROR(VLOOKUP($B18, ZEN!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B18, ZEN_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B18, CLM!$B$2:$D$101, 2,FALSE), 0)+ IFERROR(VLOOKUP($B18, CLM_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B18, THUNDER!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B18, THUNDER_3200!$B$2:$D$101, 2,FALSE), 0)</f>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D18" s="78">
         <f>IFERROR(VLOOKUP($B18, ZEN!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B18, ZEN_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B18, CLM!$B$2:$D$101, 3,FALSE), 0)+ IFERROR(VLOOKUP($B18, CLM_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B18, THUNDER!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B18, THUNDER_3200!$B$2:$D$101, 3,FALSE), 0)</f>
@@ -15228,23 +15232,23 @@
       </c>
       <c r="E18" s="79">
         <f t="shared" si="5"/>
-        <v>0.13793103448275862</v>
+        <v>0.13559322033898305</v>
       </c>
       <c r="F18" s="79">
         <f>(E18 + Params!$B$3^2/(2 * C18))/(1 + Params!$B$3^2/C18)</f>
-        <v>0.16042275749657187</v>
+        <v>0.15786994602301663</v>
       </c>
       <c r="G18" s="80">
         <f>IFERROR((Params!$B$3/(1+Params!$B$3^2/C18))*SQRT(E18*(1-E18)/C18 + (Params!$B$3/(2*C18))^2), 0)</f>
-        <v>8.8838741231750035E-2</v>
+        <v>8.7529038526160952E-2</v>
       </c>
       <c r="H18" s="80">
         <f t="shared" si="1"/>
-        <v>7.1584016264821831E-2</v>
+        <v>7.0340907496855676E-2</v>
       </c>
       <c r="I18" s="81">
         <f t="shared" si="2"/>
-        <v>0.2492614987283219</v>
+        <v>0.24539898454917758</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -15256,31 +15260,31 @@
       </c>
       <c r="C19" s="20">
         <f>IFERROR(VLOOKUP($B19, ZEN!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B19, ZEN_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B19, CLM!$B$2:$D$101, 2,FALSE), 0)+ IFERROR(VLOOKUP($B19, CLM_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B19, THUNDER!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B19, THUNDER_3200!$B$2:$D$101, 2,FALSE), 0)</f>
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D19" s="20">
         <f>IFERROR(VLOOKUP($B19, ZEN!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B19, ZEN_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B19, CLM!$B$2:$D$101, 3,FALSE), 0)+ IFERROR(VLOOKUP($B19, CLM_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B19, THUNDER!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B19, THUNDER_3200!$B$2:$D$101, 3,FALSE), 0)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E19" s="54">
         <f t="shared" si="5"/>
-        <v>0.38596491228070173</v>
+        <v>0.39655172413793105</v>
       </c>
       <c r="F19" s="54">
         <f>(E19 + Params!$B$3^2/(2 * C19))/(1 + Params!$B$3^2/C19)</f>
-        <v>0.39316520275600902</v>
+        <v>0.40297793071330623</v>
       </c>
       <c r="G19" s="21">
         <f>IFERROR((Params!$B$3/(1+Params!$B$3^2/C19))*SQRT(E19*(1-E19)/C19 + (Params!$B$3/(2*C19))^2), 0)</f>
-        <v>0.12253983280076193</v>
+        <v>0.1220922412121949</v>
       </c>
       <c r="H19" s="21">
         <f t="shared" si="1"/>
-        <v>0.27062536995524711</v>
+        <v>0.28088568950111131</v>
       </c>
       <c r="I19" s="47">
         <f t="shared" si="2"/>
-        <v>0.51570503555677094</v>
+        <v>0.52507017192550109</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -15328,7 +15332,7 @@
       </c>
       <c r="C21" s="24">
         <f>IFERROR(VLOOKUP($B21, ZEN!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B21, ZEN_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B21, CLM!$B$2:$D$101, 2,FALSE), 0)+ IFERROR(VLOOKUP($B21, CLM_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B21, THUNDER!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B21, THUNDER_3200!$B$2:$D$101, 2,FALSE), 0)</f>
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D21" s="24">
         <f>IFERROR(VLOOKUP($B21, ZEN!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B21, ZEN_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B21, CLM!$B$2:$D$101, 3,FALSE), 0)+ IFERROR(VLOOKUP($B21, CLM_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B21, THUNDER!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B21, THUNDER_3200!$B$2:$D$101, 3,FALSE), 0)</f>
@@ -15336,23 +15340,23 @@
       </c>
       <c r="E21" s="55">
         <f t="shared" si="5"/>
-        <v>0.39743589743589741</v>
+        <v>0.39240506329113922</v>
       </c>
       <c r="F21" s="55">
         <f>(E21 + Params!$B$3^2/(2 * C21))/(1 + Params!$B$3^2/C21)</f>
-        <v>0.4022502003870892</v>
+        <v>0.39739454573547589</v>
       </c>
       <c r="G21" s="25">
         <f>IFERROR((Params!$B$3/(1+Params!$B$3^2/C21))*SQRT(E21*(1-E21)/C21 + (Params!$B$3/(2*C21))^2), 0)</f>
-        <v>0.10613324782920337</v>
+        <v>0.10526756906167181</v>
       </c>
       <c r="H21" s="25">
         <f t="shared" si="1"/>
-        <v>0.29611695255788584</v>
+        <v>0.29212697667380405</v>
       </c>
       <c r="I21" s="48">
         <f t="shared" si="2"/>
-        <v>0.50838344821629255</v>
+        <v>0.50266211479714773</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -15364,31 +15368,31 @@
       </c>
       <c r="C22" s="85">
         <f>IFERROR(VLOOKUP($B22, ZEN!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B22, ZEN_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B22, CLM!$B$2:$D$101, 2,FALSE), 0)+ IFERROR(VLOOKUP($B22, CLM_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B22, THUNDER!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B22, THUNDER_3200!$B$2:$D$101, 2,FALSE), 0)</f>
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="D22" s="85">
         <f>IFERROR(VLOOKUP($B22, ZEN!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B22, ZEN_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B22, CLM!$B$2:$D$101, 3,FALSE), 0)+ IFERROR(VLOOKUP($B22, CLM_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B22, THUNDER!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B22, THUNDER_3200!$B$2:$D$101, 3,FALSE), 0)</f>
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E22" s="86">
         <f t="shared" ref="E22:E29" si="7">IFERROR(D22/C22, 0)</f>
-        <v>0.44444444444444442</v>
+        <v>0.44</v>
       </c>
       <c r="F22" s="86">
         <f>(E22 + Params!$B$3^2/(2 * C22))/(1 + Params!$B$3^2/C22)</f>
-        <v>0.44763739946380693</v>
+        <v>0.44292353275428198</v>
       </c>
       <c r="G22" s="87">
         <f>IFERROR((Params!$B$3/(1+Params!$B$3^2/C22))*SQRT(E22*(1-E22)/C22 + (Params!$B$3/(2*C22))^2), 0)</f>
-        <v>0.11916839412748018</v>
+        <v>0.10961077298643349</v>
       </c>
       <c r="H22" s="87">
         <f t="shared" si="1"/>
-        <v>0.32846900533632672</v>
+        <v>0.33331275976784847</v>
       </c>
       <c r="I22" s="88">
         <f t="shared" si="2"/>
-        <v>0.56680579359128713</v>
+        <v>0.55253430574071549</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -15400,11 +15404,11 @@
       </c>
       <c r="C23" s="73">
         <f>IFERROR(VLOOKUP($B23, ZEN!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B23, ZEN_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B23, CLM!$B$2:$D$101, 2,FALSE), 0)+ IFERROR(VLOOKUP($B23, CLM_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B23, THUNDER!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B23, THUNDER_3200!$B$2:$D$101, 2,FALSE), 0)</f>
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D23" s="73">
         <f>IFERROR(VLOOKUP($B23, ZEN!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B23, ZEN_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B23, CLM!$B$2:$D$101, 3,FALSE), 0)+ IFERROR(VLOOKUP($B23, CLM_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B23, THUNDER!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B23, THUNDER_3200!$B$2:$D$101, 3,FALSE), 0)</f>
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E23" s="74">
         <f t="shared" si="7"/>
@@ -15412,19 +15416,19 @@
       </c>
       <c r="F23" s="74">
         <f>(E23 + Params!$B$3^2/(2 * C23))/(1 + Params!$B$3^2/C23)</f>
-        <v>0.40601739304779333</v>
+        <v>0.40487255459047</v>
       </c>
       <c r="G23" s="75">
         <f>IFERROR((Params!$B$3/(1+Params!$B$3^2/C23))*SQRT(E23*(1-E23)/C23 + (Params!$B$3/(2*C23))^2), 0)</f>
-        <v>0.12032436301013825</v>
+        <v>0.10824912380876403</v>
       </c>
       <c r="H23" s="75">
         <f t="shared" si="1"/>
-        <v>0.28569303003765506</v>
+        <v>0.29662343078170594</v>
       </c>
       <c r="I23" s="76">
         <f t="shared" si="2"/>
-        <v>0.52634175605793154</v>
+        <v>0.51312167839923406</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -15436,31 +15440,31 @@
       </c>
       <c r="C24" s="24">
         <f>IFERROR(VLOOKUP($B24, ZEN!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B24, ZEN_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B24, CLM!$B$2:$D$101, 2,FALSE), 0)+ IFERROR(VLOOKUP($B24, CLM_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B24, THUNDER!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B24, THUNDER_3200!$B$2:$D$101, 2,FALSE), 0)</f>
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D24" s="24">
         <f>IFERROR(VLOOKUP($B24, ZEN!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B24, ZEN_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B24, CLM!$B$2:$D$101, 3,FALSE), 0)+ IFERROR(VLOOKUP($B24, CLM_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B24, THUNDER!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B24, THUNDER_3200!$B$2:$D$101, 3,FALSE), 0)</f>
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E24" s="55">
         <f t="shared" si="7"/>
-        <v>0.532258064516129</v>
+        <v>0.54666666666666663</v>
       </c>
       <c r="F24" s="55">
         <f>(E24 + Params!$B$3^2/(2 * C24))/(1 + Params!$B$3^2/C24)</f>
-        <v>0.53037593254112902</v>
+        <v>0.54439280785778066</v>
       </c>
       <c r="G24" s="25">
         <f>IFERROR((Params!$B$3/(1+Params!$B$3^2/C24))*SQRT(E24*(1-E24)/C24 + (Params!$B$3/(2*C24))^2), 0)</f>
-        <v>0.12053775878264891</v>
+        <v>0.10991107086629816</v>
       </c>
       <c r="H24" s="25">
         <f t="shared" si="1"/>
-        <v>0.40983817375848008</v>
+        <v>0.43448173699148251</v>
       </c>
       <c r="I24" s="48">
         <f t="shared" si="2"/>
-        <v>0.65091369132377797</v>
+        <v>0.6543038787240788</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -15508,31 +15512,31 @@
       </c>
       <c r="C26" s="106">
         <f>IFERROR(VLOOKUP($B26, ZEN!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B26, ZEN_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B26, CLM!$B$2:$D$101, 2,FALSE), 0)+ IFERROR(VLOOKUP($B26, CLM_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B26, THUNDER!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B26, THUNDER_3200!$B$2:$D$101, 2,FALSE), 0)</f>
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="D26" s="106">
         <f>IFERROR(VLOOKUP($B26, ZEN!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B26, ZEN_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B26, CLM!$B$2:$D$101, 3,FALSE), 0)+ IFERROR(VLOOKUP($B26, CLM_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B26, THUNDER!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B26, THUNDER_3200!$B$2:$D$101, 3,FALSE), 0)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E26" s="107">
         <f t="shared" si="7"/>
-        <v>0.24193548387096775</v>
+        <v>0.21621621621621623</v>
       </c>
       <c r="F26" s="107">
         <f>(E26 + Params!$B$3^2/(2 * C26))/(1 + Params!$B$3^2/C26)</f>
-        <v>0.25699253967096797</v>
+        <v>0.23022137263365605</v>
       </c>
       <c r="G26" s="108">
         <f>IFERROR((Params!$B$3/(1+Params!$B$3^2/C26))*SQRT(E26*(1-E26)/C26 + (Params!$B$3/(2*C26))^2), 0)</f>
-        <v>0.10453490286148255</v>
+        <v>9.2518019959391004E-2</v>
       </c>
       <c r="H26" s="108">
         <f t="shared" si="1"/>
-        <v>0.15245763680948543</v>
+        <v>0.13770335267426503</v>
       </c>
       <c r="I26" s="109">
         <f t="shared" si="2"/>
-        <v>0.3615274425324505</v>
+        <v>0.32273939259304707</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -15544,31 +15548,31 @@
       </c>
       <c r="C27" s="106">
         <f>IFERROR(VLOOKUP($B27, ZEN!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B27, ZEN_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B27, CLM!$B$2:$D$101, 2,FALSE), 0)+ IFERROR(VLOOKUP($B27, CLM_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B27, THUNDER!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B27, THUNDER_3200!$B$2:$D$101, 2,FALSE), 0)</f>
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D27" s="106">
         <f>IFERROR(VLOOKUP($B27, ZEN!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B27, ZEN_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B27, CLM!$B$2:$D$101, 3,FALSE), 0)+ IFERROR(VLOOKUP($B27, CLM_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B27, THUNDER!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B27, THUNDER_3200!$B$2:$D$101, 3,FALSE), 0)</f>
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E27" s="107">
         <f t="shared" si="7"/>
-        <v>0.40322580645161288</v>
+        <v>0.41333333333333333</v>
       </c>
       <c r="F27" s="107">
         <f>(E27 + Params!$B$3^2/(2 * C27))/(1 + Params!$B$3^2/C27)</f>
-        <v>0.40887220237661298</v>
+        <v>0.41755621397840731</v>
       </c>
       <c r="G27" s="108">
         <f>IFERROR((Params!$B$3/(1+Params!$B$3^2/C27))*SQRT(E27*(1-E27)/C27 + (Params!$B$3/(2*C27))^2), 0)</f>
-        <v>0.11862537326008812</v>
+        <v>0.10878067938691047</v>
       </c>
       <c r="H27" s="108">
         <f t="shared" si="1"/>
-        <v>0.29024682911652488</v>
+        <v>0.30877553459149687</v>
       </c>
       <c r="I27" s="109">
         <f t="shared" si="2"/>
-        <v>0.52749757563670108</v>
+        <v>0.52633689336531775</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -15580,31 +15584,31 @@
       </c>
       <c r="C28" s="106">
         <f>IFERROR(VLOOKUP($B28, ZEN!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B28, ZEN_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B28, CLM!$B$2:$D$101, 2,FALSE), 0)+ IFERROR(VLOOKUP($B28, CLM_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B28, THUNDER!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B28, THUNDER_3200!$B$2:$D$101, 2,FALSE), 0)</f>
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="D28" s="106">
         <f>IFERROR(VLOOKUP($B28, ZEN!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B28, ZEN_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B28, CLM!$B$2:$D$101, 3,FALSE), 0)+ IFERROR(VLOOKUP($B28, CLM_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B28, THUNDER!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B28, THUNDER_3200!$B$2:$D$101, 3,FALSE), 0)</f>
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E28" s="107">
         <f t="shared" si="7"/>
-        <v>0.44262295081967212</v>
+        <v>0.41333333333333333</v>
       </c>
       <c r="F28" s="107">
         <f>(E28 + Params!$B$3^2/(2 * C28))/(1 + Params!$B$3^2/C28)</f>
-        <v>0.44602230666732468</v>
+        <v>0.41755621397840731</v>
       </c>
       <c r="G28" s="108">
         <f>IFERROR((Params!$B$3/(1+Params!$B$3^2/C28))*SQRT(E28*(1-E28)/C28 + (Params!$B$3/(2*C28))^2), 0)</f>
-        <v>0.12094622632812023</v>
+        <v>0.10878067938691047</v>
       </c>
       <c r="H28" s="108">
         <f t="shared" si="1"/>
-        <v>0.32507608033920443</v>
+        <v>0.30877553459149687</v>
       </c>
       <c r="I28" s="109">
         <f t="shared" si="2"/>
-        <v>0.56696853299544492</v>
+        <v>0.52633689336531775</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -15616,31 +15620,31 @@
       </c>
       <c r="C29" s="106">
         <f>IFERROR(VLOOKUP($B29, ZEN!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B29, ZEN_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B29, CLM!$B$2:$D$101, 2,FALSE), 0)+ IFERROR(VLOOKUP($B29, CLM_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B29, THUNDER!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B29, THUNDER_3200!$B$2:$D$101, 2,FALSE), 0)</f>
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="D29" s="106">
         <f>IFERROR(VLOOKUP($B29, ZEN!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B29, ZEN_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B29, CLM!$B$2:$D$101, 3,FALSE), 0)+ IFERROR(VLOOKUP($B29, CLM_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B29, THUNDER!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B29, THUNDER_3200!$B$2:$D$101, 3,FALSE), 0)</f>
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E29" s="107">
         <f t="shared" si="7"/>
-        <v>0.60655737704918034</v>
+        <v>0.6</v>
       </c>
       <c r="F29" s="107">
         <f>(E29 + Params!$B$3^2/(2 * C29))/(1 + Params!$B$3^2/C29)</f>
-        <v>0.60024428761782556</v>
+        <v>0.59512744540953</v>
       </c>
       <c r="G29" s="108">
         <f>IFERROR((Params!$B$3/(1+Params!$B$3^2/C29))*SQRT(E29*(1-E29)/C29 + (Params!$B$3/(2*C29))^2), 0)</f>
-        <v>0.11907404376173815</v>
+        <v>0.10824912380876403</v>
       </c>
       <c r="H29" s="108">
         <f t="shared" si="1"/>
-        <v>0.48117024385608742</v>
+        <v>0.48687832160076594</v>
       </c>
       <c r="I29" s="109">
         <f t="shared" si="2"/>
-        <v>0.71931833137956369</v>
+        <v>0.70337656921829406</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -15688,7 +15692,7 @@
       </c>
       <c r="C31" s="58">
         <f>IFERROR(VLOOKUP($B31, ZEN!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B31, ZEN_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B31, CLM!$B$2:$D$101, 2,FALSE), 0)+ IFERROR(VLOOKUP($B31, CLM_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B31, THUNDER!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B31, THUNDER_3200!$B$2:$D$101, 2,FALSE), 0)</f>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D31" s="58">
         <f>IFERROR(VLOOKUP($B31, ZEN!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B31, ZEN_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B31, CLM!$B$2:$D$101, 3,FALSE), 0)+ IFERROR(VLOOKUP($B31, CLM_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B31, THUNDER!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B31, THUNDER_3200!$B$2:$D$101, 3,FALSE), 0)</f>
@@ -15696,23 +15700,23 @@
       </c>
       <c r="E31" s="59">
         <f t="shared" si="5"/>
-        <v>0.15517241379310345</v>
+        <v>0.15254237288135594</v>
       </c>
       <c r="F31" s="59">
         <f>(E31 + Params!$B$3^2/(2 * C31))/(1 + Params!$B$3^2/C31)</f>
-        <v>0.17659310237768752</v>
+        <v>0.17378297178938795</v>
       </c>
       <c r="G31" s="60">
         <f>IFERROR((Params!$B$3/(1+Params!$B$3^2/C31))*SQRT(E31*(1-E31)/C31 + (Params!$B$3/(2*C31))^2), 0)</f>
-        <v>9.2749128210185508E-2</v>
+        <v>9.1399260898714321E-2</v>
       </c>
       <c r="H31" s="60">
         <f t="shared" si="1"/>
-        <v>8.3843974167502014E-2</v>
+        <v>8.2383710890673631E-2</v>
       </c>
       <c r="I31" s="61">
         <f t="shared" si="2"/>
-        <v>0.26934223058787304</v>
+        <v>0.26518223268810226</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -15760,31 +15764,31 @@
       </c>
       <c r="C33" s="111">
         <f>IFERROR(VLOOKUP($B33, ZEN!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B33, ZEN_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B33, CLM!$B$2:$D$101, 2,FALSE), 0)+ IFERROR(VLOOKUP($B33, CLM_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B33, THUNDER!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B33, THUNDER_3200!$B$2:$D$101, 2,FALSE), 0)</f>
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D33" s="111">
         <f>IFERROR(VLOOKUP($B33, ZEN!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B33, ZEN_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B33, CLM!$B$2:$D$101, 3,FALSE), 0)+ IFERROR(VLOOKUP($B33, CLM_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B33, THUNDER!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B33, THUNDER_3200!$B$2:$D$101, 3,FALSE), 0)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E33" s="112">
         <f t="shared" si="5"/>
-        <v>0.14285714285714285</v>
+        <v>0.16981132075471697</v>
       </c>
       <c r="F33" s="112">
         <f>(E33 + Params!$B$3^2/(2 * C33))/(1 + Params!$B$3^2/C33)</f>
-        <v>0.16882153454853752</v>
+        <v>0.19212689297978941</v>
       </c>
       <c r="G33" s="113">
         <f>IFERROR((Params!$B$3/(1+Params!$B$3^2/C33))*SQRT(E33*(1-E33)/C33 + (Params!$B$3/(2*C33))^2), 0)</f>
-        <v>9.7858197343091674E-2</v>
+        <v>0.10012847525755188</v>
       </c>
       <c r="H33" s="113">
         <f t="shared" si="1"/>
-        <v>7.0963337205445842E-2</v>
+        <v>9.1998417722237533E-2</v>
       </c>
       <c r="I33" s="114">
         <f t="shared" si="2"/>
-        <v>0.26667973189162919</v>
+        <v>0.29225536823734127</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -15796,7 +15800,7 @@
       </c>
       <c r="C34" s="111">
         <f>IFERROR(VLOOKUP($B34, ZEN!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B34, ZEN_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B34, CLM!$B$2:$D$101, 2,FALSE), 0)+ IFERROR(VLOOKUP($B34, CLM_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B34, THUNDER!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B34, THUNDER_3200!$B$2:$D$101, 2,FALSE), 0)</f>
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D34" s="111">
         <f>IFERROR(VLOOKUP($B34, ZEN!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B34, ZEN_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B34, CLM!$B$2:$D$101, 3,FALSE), 0)+ IFERROR(VLOOKUP($B34, CLM_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B34, THUNDER!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B34, THUNDER_3200!$B$2:$D$101, 3,FALSE), 0)</f>
@@ -15804,23 +15808,23 @@
       </c>
       <c r="E34" s="112">
         <f t="shared" ref="E34:E35" si="10">IFERROR(D34/C34, 0)</f>
-        <v>0.1702127659574468</v>
+        <v>0.15094339622641509</v>
       </c>
       <c r="F34" s="112">
         <f>(E34 + Params!$B$3^2/(2 * C34))/(1 + Params!$B$3^2/C34)</f>
-        <v>0.19513154582074524</v>
+        <v>0.17453414400720596</v>
       </c>
       <c r="G34" s="113">
         <f>IFERROR((Params!$B$3/(1+Params!$B$3^2/C34))*SQRT(E34*(1-E34)/C34 + (Params!$B$3/(2*C34))^2), 0)</f>
-        <v>0.10626896490810595</v>
+        <v>9.601090142938945E-2</v>
       </c>
       <c r="H34" s="113">
         <f t="shared" si="1"/>
-        <v>8.8862580912639294E-2</v>
+        <v>7.852324257781651E-2</v>
       </c>
       <c r="I34" s="114">
         <f t="shared" si="2"/>
-        <v>0.30140051072885121</v>
+        <v>0.27054504543659541</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -15832,31 +15836,31 @@
       </c>
       <c r="C35" s="63">
         <f>IFERROR(VLOOKUP($B35, ZEN!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B35, ZEN_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B35, CLM!$B$2:$D$101, 2,FALSE), 0)+ IFERROR(VLOOKUP($B35, CLM_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B35, THUNDER!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B35, THUNDER_3200!$B$2:$D$101, 2,FALSE), 0)</f>
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="D35" s="63">
         <f>IFERROR(VLOOKUP($B35, ZEN!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B35, ZEN_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B35, CLM!$B$2:$D$101, 3,FALSE), 0)+ IFERROR(VLOOKUP($B35, CLM_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B35, THUNDER!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B35, THUNDER_3200!$B$2:$D$101, 3,FALSE), 0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35" s="64">
         <f t="shared" si="10"/>
-        <v>2.0833333333333332E-2</v>
+        <v>3.7735849056603772E-2</v>
       </c>
       <c r="F35" s="64">
         <f>(E35 + Params!$B$3^2/(2 * C35))/(1 + Params!$B$3^2/C35)</f>
-        <v>5.6340853677355633E-2</v>
+        <v>6.8977650171705207E-2</v>
       </c>
       <c r="G35" s="65">
         <f>IFERROR((Params!$B$3/(1+Params!$B$3^2/C35))*SQRT(E35*(1-E35)/C35 + (Params!$B$3/(2*C35))^2), 0)</f>
-        <v>5.2653837697955938E-2</v>
+        <v>5.8567581337885935E-2</v>
       </c>
       <c r="H35" s="65">
         <f t="shared" si="1"/>
-        <v>3.6870159793996951E-3</v>
+        <v>1.0410068833819272E-2</v>
       </c>
       <c r="I35" s="66">
         <f t="shared" si="2"/>
-        <v>0.10899469137531156</v>
+        <v>0.12754523150959113</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -15868,7 +15872,7 @@
       </c>
       <c r="C36" s="63">
         <f>IFERROR(VLOOKUP($B36, ZEN!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B36, ZEN_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B36, CLM!$B$2:$D$101, 2,FALSE), 0)+ IFERROR(VLOOKUP($B36, CLM_3200!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B36, THUNDER!$B$2:$D$101, 2,FALSE), 0) + IFERROR(VLOOKUP($B36, THUNDER_3200!$B$2:$D$101, 2,FALSE), 0)</f>
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D36" s="63">
         <f>IFERROR(VLOOKUP($B36, ZEN!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B36, ZEN_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B36, CLM!$B$2:$D$101, 3,FALSE), 0)+ IFERROR(VLOOKUP($B36, CLM_3200!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B36, THUNDER!$B$2:$D$101, 3,FALSE), 0) + IFERROR(VLOOKUP($B36, THUNDER_3200!$B$2:$D$101, 3,FALSE), 0)</f>
@@ -15876,23 +15880,23 @@
       </c>
       <c r="E36" s="64">
         <f t="shared" ref="E36" si="11">IFERROR(D36/C36, 0)</f>
-        <v>2.1276595744680851E-2</v>
+        <v>1.8867924528301886E-2</v>
       </c>
       <c r="F36" s="64">
         <f>(E36 + Params!$B$3^2/(2 * C36))/(1 + Params!$B$3^2/C36)</f>
-        <v>5.7449018126888213E-2</v>
+        <v>5.1384901199121757E-2</v>
       </c>
       <c r="G36" s="65">
         <f>IFERROR((Params!$B$3/(1+Params!$B$3^2/C36))*SQRT(E36*(1-E36)/C36 + (Params!$B$3/(2*C36))^2), 0)</f>
-        <v>5.3683347116423218E-2</v>
+        <v>4.8046533812372359E-2</v>
       </c>
       <c r="H36" s="65">
         <f t="shared" si="1"/>
-        <v>3.7656710104649951E-3</v>
+        <v>3.3383673867493982E-3</v>
       </c>
       <c r="I36" s="66">
         <f t="shared" si="2"/>
-        <v>0.11113236524331144</v>
+        <v>9.9431435011494124E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>